<commit_message>
14 Jan 2021: True False done; Fill ups done; matchup done;
</commit_message>
<xml_diff>
--- a/mytests/xlsdocs/Fillups.xlsx
+++ b/mytests/xlsdocs/Fillups.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>Module</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +422,7 @@
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -532,9 +533,85 @@
         <v>21</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
         <v>171</v>
       </c>
     </row>

</xml_diff>